<commit_message>
Se modificó el archivo de excel
</commit_message>
<xml_diff>
--- a/CASOS DE PRUEBA PROYECTO.xlsx
+++ b/CASOS DE PRUEBA PROYECTO.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27932"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b14s205\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A869F9C-4414-4C06-A874-87FA02BA6123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -22,6 +28,9 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -158,14 +167,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,346 +184,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="12">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -565,255 +238,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -847,90 +278,165 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Coma" xfId="1" builtinId="3"/>
-    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
-    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
-    <cellStyle name="Coma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Moneda [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hipervínculo" xfId="6" builtinId="8"/>
-    <cellStyle name="Hipervínculo visitado" xfId="7" builtinId="9"/>
-    <cellStyle name="Nota" xfId="8" builtinId="10"/>
-    <cellStyle name="Texto de advertencia" xfId="9" builtinId="11"/>
-    <cellStyle name="Título" xfId="10" builtinId="15"/>
-    <cellStyle name="Texto explicativo" xfId="11" builtinId="53"/>
-    <cellStyle name="Título 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Título 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Título 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Título 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Entrada" xfId="16" builtinId="20"/>
-    <cellStyle name="Salida" xfId="17" builtinId="21"/>
-    <cellStyle name="Cálculo" xfId="18" builtinId="22"/>
-    <cellStyle name="Celda de comprobación" xfId="19" builtinId="23"/>
-    <cellStyle name="Celda vinculada" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Correcto" xfId="22" builtinId="26"/>
-    <cellStyle name="Incorrecto" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutro" xfId="24" builtinId="28"/>
-    <cellStyle name="Énfasis1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Énfasis1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Énfasis1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Énfasis1" xfId="28" builtinId="32"/>
-    <cellStyle name="Énfasis2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Énfasis2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Énfasis2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Énfasis2" xfId="32" builtinId="36"/>
-    <cellStyle name="Énfasis3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Énfasis3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Énfasis3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Énfasis3" xfId="36" builtinId="40"/>
-    <cellStyle name="Énfasis4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Énfasis4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Énfasis4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Énfasis4" xfId="40" builtinId="44"/>
-    <cellStyle name="Énfasis5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Énfasis5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Énfasis5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Énfasis5" xfId="44" builtinId="48"/>
-    <cellStyle name="Énfasis6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Énfasis6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Énfasis6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Énfasis6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79995117038483843"/>
+          <bgColor theme="4" tint="0.79995117038483843"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="1"/>
       </font>
       <border>
@@ -941,7 +447,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="1"/>
+        <b/>
         <color theme="0"/>
       </font>
       <fill>
@@ -969,154 +475,40 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.399975585192419"/>
+          <color theme="4" tint="0.39994506668294322"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="1"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.799981688894314"/>
-          <bgColor theme="4" tint="0.799981688894314"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.399975585192419"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="6"/>
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="totalRow" dxfId="4"/>
-      <tableStyleElement type="firstColumn" dxfId="3"/>
-      <tableStyleElement type="lastColumn" dxfId="2"/>
-      <tableStyleElement type="firstRowStripe" dxfId="1"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
+      <tableStyleElement type="lastColumn" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
-      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+      <tableStyleElement type="headerRow" dxfId="9"/>
+      <tableStyleElement type="totalRow" dxfId="8"/>
+      <tableStyleElement type="firstRowStripe" dxfId="7"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
+      <tableStyleElement type="pageFieldValues" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1374,39 +766,38 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:O22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.5714285714286" customWidth="1"/>
-    <col min="2" max="2" width="12.8571428571429" customWidth="1"/>
-    <col min="3" max="3" width="12.7142857142857" customWidth="1"/>
+    <col min="1" max="1" width="30.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
-    <col min="5" max="5" width="12.1428571428571" customWidth="1"/>
-    <col min="6" max="6" width="8.71428571428571" customWidth="1"/>
-    <col min="7" max="7" width="20.5714285714286" customWidth="1"/>
-    <col min="8" max="8" width="6.42857142857143" customWidth="1"/>
-    <col min="9" max="9" width="8.71428571428571" customWidth="1"/>
-    <col min="10" max="10" width="18.7142857142857" customWidth="1"/>
-    <col min="11" max="11" width="13.7142857142857" customWidth="1"/>
-    <col min="12" max="12" width="16.2857142857143" customWidth="1"/>
-    <col min="13" max="13" width="11.7142857142857" customWidth="1"/>
-    <col min="14" max="14" width="12.8571428571429" customWidth="1"/>
-    <col min="15" max="15" width="52.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="16.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="52.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75"/>
-    <row r="2" ht="90" spans="6:10">
+    <row r="2" spans="1:15" ht="90">
       <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1419,26 +810,26 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" ht="30" spans="1:15">
+    <row r="4" spans="1:15" ht="30">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1501,7 +892,9 @@
       <c r="E5" s="3">
         <v>100000</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3">
+        <v>0</v>
+      </c>
       <c r="G5" s="3">
         <f>B5+C5+D5+E5+F5</f>
         <v>5300000</v>
@@ -1553,7 +946,9 @@
       <c r="E6" s="3">
         <v>20000</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G22" si="0">B6+C6+D6+E6+F6</f>
         <v>6420000</v>
@@ -1605,7 +1000,9 @@
       <c r="E7" s="3">
         <v>20000</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>4620000</v>
@@ -1657,7 +1054,9 @@
       <c r="E8" s="3">
         <v>10000</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>4270000</v>
@@ -1702,7 +1101,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="8"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -1721,7 +1120,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="3"/>
+      <c r="I10" s="8"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -1755,9 +1154,11 @@
       <c r="H11" s="8">
         <v>0.04</v>
       </c>
-      <c r="I11" s="3"/>
+      <c r="I11" s="8">
+        <v>0.04</v>
+      </c>
       <c r="J11" s="3">
-        <f t="shared" ref="J6:J22" si="5">IF(B11&gt;2*G8,B11*1%,0)</f>
+        <f t="shared" ref="J11:J22" si="5">IF(B11&gt;2*G8,B11*1%,0)</f>
         <v>0</v>
       </c>
       <c r="K11" s="3">
@@ -1777,21 +1178,29 @@
         <v>0</v>
       </c>
       <c r="O11" s="3">
-        <f t="shared" ref="O9:O14" si="6">N11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" ht="30" spans="1:15">
+        <f t="shared" ref="O11:O14" si="6">N11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="30">
       <c r="A12" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B12" s="3">
         <v>3500000</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
       <c r="G12" s="3">
         <f t="shared" si="0"/>
         <v>3500000</v>
@@ -1799,7 +1208,9 @@
       <c r="H12" s="8">
         <v>0.04</v>
       </c>
-      <c r="I12" s="3"/>
+      <c r="I12" s="8">
+        <v>0.04</v>
+      </c>
       <c r="J12" s="3">
         <f t="shared" si="5"/>
         <v>35000</v>
@@ -1810,19 +1221,19 @@
       </c>
       <c r="L12" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>140000</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="3"/>
-        <v>175000</v>
+        <v>315000</v>
       </c>
       <c r="N12" s="3">
         <f t="shared" si="4"/>
-        <v>3325000</v>
+        <v>3185000</v>
       </c>
       <c r="O12" s="3">
         <f t="shared" si="6"/>
-        <v>3325000</v>
+        <v>3185000</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1841,7 +1252,9 @@
       <c r="E13" s="3">
         <v>30000</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
       <c r="G13" s="3">
         <f t="shared" si="0"/>
         <v>25330000</v>
@@ -1849,7 +1262,9 @@
       <c r="H13" s="8">
         <v>0.04</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="8">
+        <v>0.04</v>
+      </c>
       <c r="J13" s="3">
         <f t="shared" si="5"/>
         <v>250000</v>
@@ -1860,29 +1275,37 @@
       </c>
       <c r="L13" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1000000</v>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="3"/>
-        <v>1250000</v>
+        <v>2250000</v>
       </c>
       <c r="N13" s="3">
         <f t="shared" si="4"/>
-        <v>24080000</v>
+        <v>23080000</v>
       </c>
       <c r="O13" s="3">
         <f t="shared" si="6"/>
-        <v>24080000</v>
+        <v>23080000</v>
       </c>
     </row>
     <row r="14" spans="1:15">
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="3">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
       <c r="F14" s="3">
         <v>249095</v>
       </c>
@@ -1893,7 +1316,9 @@
       <c r="H14" s="8">
         <v>0.04</v>
       </c>
-      <c r="I14" s="3"/>
+      <c r="I14" s="8">
+        <v>0.04</v>
+      </c>
       <c r="J14" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -1926,34 +1351,14 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="8">
-        <v>0.04</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="3">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N15" s="3">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
       <c r="O15" s="3"/>
     </row>
     <row r="16" spans="1:15">
@@ -1967,7 +1372,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="3"/>
+      <c r="I16" s="8"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
@@ -1982,10 +1387,18 @@
       <c r="B17" s="3">
         <v>-200000</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="C17" s="3">
+        <v>0</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
       <c r="G17" s="3">
         <f t="shared" si="0"/>
         <v>-200000</v>
@@ -1993,7 +1406,9 @@
       <c r="H17" s="8">
         <v>0.04</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="I17" s="8">
+        <v>0.04</v>
+      </c>
       <c r="J17" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2004,15 +1419,15 @@
       </c>
       <c r="L17" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-8000</v>
       </c>
       <c r="M17" s="3">
         <f t="shared" si="3"/>
-        <v>-8000</v>
+        <v>-16000</v>
       </c>
       <c r="N17" s="3">
         <f t="shared" si="4"/>
-        <v>-192000</v>
+        <v>-184000</v>
       </c>
       <c r="O17" s="3" t="s">
         <v>29</v>
@@ -2025,10 +1440,18 @@
       <c r="B18" s="3">
         <v>99999999999</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
       <c r="G18" s="3">
         <f t="shared" si="0"/>
         <v>99999999999</v>
@@ -2036,10 +1459,12 @@
       <c r="H18" s="8">
         <v>0.04</v>
       </c>
-      <c r="I18" s="3"/>
+      <c r="I18" s="8">
+        <v>0.04</v>
+      </c>
       <c r="J18" s="3">
         <f t="shared" si="5"/>
-        <v>999999999.99</v>
+        <v>999999999.99000001</v>
       </c>
       <c r="K18" s="3">
         <f t="shared" si="1"/>
@@ -2047,15 +1472,15 @@
       </c>
       <c r="L18" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3999999999.96</v>
       </c>
       <c r="M18" s="3">
         <f t="shared" si="3"/>
-        <v>4999999999.95</v>
+        <v>8999999999.9099998</v>
       </c>
       <c r="N18" s="3">
         <f t="shared" si="4"/>
-        <v>94999999999.05</v>
+        <v>90999999999.089996</v>
       </c>
       <c r="O18" s="3" t="s">
         <v>31</v>
@@ -2077,7 +1502,9 @@
       <c r="E19" s="3">
         <v>34500</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
       <c r="G19" s="3" t="e">
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
@@ -2085,7 +1512,9 @@
       <c r="H19" s="8">
         <v>0.04</v>
       </c>
-      <c r="I19" s="3"/>
+      <c r="I19" s="8">
+        <v>0.04</v>
+      </c>
       <c r="J19" s="3" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
@@ -2124,7 +1553,9 @@
       <c r="E20" s="3">
         <v>60000</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
       <c r="G20" s="3">
         <f t="shared" si="0"/>
         <v>134500</v>
@@ -2132,7 +1563,9 @@
       <c r="H20" s="8">
         <v>0.04</v>
       </c>
-      <c r="I20" s="3"/>
+      <c r="I20" s="8">
+        <v>0.04</v>
+      </c>
       <c r="J20" s="3">
         <f t="shared" si="5"/>
         <v>0</v>
@@ -2164,29 +1597,39 @@
       <c r="B21" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3" t="e">
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3">
         <f t="shared" si="0"/>
-        <v>#VALUE!</v>
+        <v>1500.75</v>
       </c>
       <c r="H21" s="8">
         <v>0.04</v>
       </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3" t="e">
+      <c r="I21" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="J21" s="3">
         <f t="shared" si="5"/>
-        <v>#VALUE!</v>
+        <v>15.0075</v>
       </c>
       <c r="K21" s="3" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L21" s="3" t="e">
+      <c r="L21" s="3">
         <f t="shared" si="2"/>
-        <v>#VALUE!</v>
+        <v>60.03</v>
       </c>
       <c r="M21" s="3" t="e">
         <f t="shared" si="3"/>
@@ -2216,7 +1659,9 @@
       <c r="E22" s="3">
         <v>60000</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
       <c r="G22" s="3">
         <f t="shared" si="0"/>
         <v>112001</v>
@@ -2224,7 +1669,9 @@
       <c r="H22" s="8">
         <v>0.04</v>
       </c>
-      <c r="I22" s="3"/>
+      <c r="I22" s="8">
+        <v>0.04</v>
+      </c>
       <c r="J22" s="3" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
@@ -2235,7 +1682,7 @@
       </c>
       <c r="L22" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="M22" s="3" t="e">
         <f t="shared" si="3"/>
@@ -2255,6 +1702,5 @@
     <mergeCell ref="H3:J3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>